<commit_message>
2017 Day 1 Part 2 & Day 2 (both parts)
</commit_message>
<xml_diff>
--- a/2015/Day10.xlsx
+++ b/2015/Day10.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Financial Modelling World Cup/Advent-of-Code-Excel/2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Excel/Excel &amp; Financial Modelling/Advent-of-Code-Excel/2015/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F25CC0-CB70-1642-89AC-EC6517F600FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A4D8B3-9358-9246-B9DC-1A620F58B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
+    <workbookView xWindow="7080" yWindow="9440" windowWidth="26540" windowHeight="12900" activeTab="1" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
   </bookViews>
   <sheets>
     <sheet name="Solutions" sheetId="3" r:id="rId1"/>
     <sheet name="Workings" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="input">Workings!#REF!</definedName>
+    <definedName name="input">Workings!$B$2</definedName>
     <definedName name="Number1">Workings!#REF!</definedName>
     <definedName name="Number2">Workings!#REF!</definedName>
     <definedName name="Target">Workings!#REF!</definedName>
@@ -38,6 +38,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,12 +463,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8F4387-9FD6-E241-86F1-7FFD05E57526}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="217" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1113222113</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3:K3">MID(B2,_xlfn.SEQUENCE(,LEN(B2)),1)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>3</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2</v>
+      </c>
+      <c r="H3" t="str">
+        <v>2</v>
+      </c>
+      <c r="I3" t="str">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <v>1</v>
+      </c>
+      <c r="K3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>